<commit_message>
finish debug TDS visopf
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis_base.xlsx
+++ b/bshe/VIS_opf/ieee39_vis_base.xlsx
@@ -10060,10 +10060,10 @@
         <v>0</v>
       </c>
       <c r="M3" t="str">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N3" t="str">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="O3" t="str">
         <v>0.1</v>

</xml_diff>

<commit_message>
to test tds maximum  load magnitute
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis_base.xlsx
+++ b/bshe/VIS_opf/ieee39_vis_base.xlsx
@@ -9370,7 +9370,7 @@
         <v>60</v>
       </c>
       <c r="K2" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L2" t="str">
         <v>8.06</v>
@@ -9456,7 +9456,7 @@
         <v>60</v>
       </c>
       <c r="K3" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L3" t="str">
         <v>7.16</v>
@@ -9542,7 +9542,7 @@
         <v>60</v>
       </c>
       <c r="K4" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L4" t="str">
         <v>8.72</v>
@@ -9628,7 +9628,7 @@
         <v>60</v>
       </c>
       <c r="K5" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L5" t="str">
         <v>5.2</v>
@@ -9714,7 +9714,7 @@
         <v>60</v>
       </c>
       <c r="K6" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L6" t="str">
         <v>8.28</v>
@@ -9800,7 +9800,7 @@
         <v>60</v>
       </c>
       <c r="K7" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L7" t="str">
         <v>10</v>
@@ -9983,10 +9983,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O2" t="str">
         <v>0.1</v>
@@ -10060,10 +10060,10 @@
         <v>0</v>
       </c>
       <c r="M3" t="str">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N3" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O3" t="str">
         <v>0.1</v>
@@ -10137,10 +10137,10 @@
         <v>0</v>
       </c>
       <c r="M4" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O4" t="str">
         <v>0.1</v>
@@ -10214,10 +10214,10 @@
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O5" t="str">
         <v>0.1</v>

</xml_diff>

<commit_message>
draft vis-rted for  four method
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis_base.xlsx
+++ b/bshe/VIS_opf/ieee39_vis_base.xlsx
@@ -9983,7 +9983,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" t="str">
         <v>1</v>
@@ -10060,7 +10060,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" t="str">
         <v>1</v>
@@ -10137,7 +10137,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" t="str">
         <v>1</v>
@@ -10214,7 +10214,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="str">
         <v>1</v>

</xml_diff>